<commit_message>
Facet test. Plot and KPI fixes.
</commit_message>
<xml_diff>
--- a/Shiny/Test/Data/OPXfinans_final.xlsx
+++ b/Shiny/Test/Data/OPXfinans_final.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaliehchristensen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7184215cb1ebccca/Documents/ISSSV1337/ISSSV1337-Case/Shiny/Test/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAF222F-AD5B-BC4F-9E29-D7D160ED2DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3AAF222F-AD5B-BC4F-9E29-D7D160ED2DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC7A1CE6-278D-4DE4-AAE2-3273608AB6E7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{53754C84-E169-0147-918E-884E18682F79}"/>
+    <workbookView xWindow="50" yWindow="0" windowWidth="16440" windowHeight="10740" xr2:uid="{53754C84-E169-0147-918E-884E18682F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -218,8 +218,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;NOK&quot;\ * #,##0.00_-;\-&quot;NOK&quot;\ * #,##0.00_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-&quot;NOK&quot;\ * #,##0_-;\-&quot;NOK&quot;\ * #,##0_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;NOK&quot;\ * #,##0.00_-;\-&quot;NOK&quot;\ * #,##0.00_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;NOK&quot;\ * #,##0_-;\-&quot;NOK&quot;\ * #,##0_-;_-&quot;NOK&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -323,7 +323,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
@@ -336,24 +336,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -667,11 +667,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22AE676F-2AEC-6041-849D-D057AD5F77E1}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -681,7 +681,7 @@
     <col min="6" max="6" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -718,7 +718,7 @@
         <v>462196</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -735,7 +735,7 @@
         <v>29148</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -752,7 +752,7 @@
         <v>4806</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -769,7 +769,7 @@
         <v>25087</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2020</v>
       </c>
@@ -803,7 +803,7 @@
         <v>81052</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2020</v>
       </c>
@@ -820,7 +820,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -837,7 +837,7 @@
         <v>434431</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -854,7 +854,7 @@
         <v>10528</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2020</v>
       </c>
@@ -871,7 +871,7 @@
         <v>93587</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -888,7 +888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2020</v>
       </c>
@@ -908,7 +908,7 @@
         <v>15691</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -928,7 +928,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2020</v>
       </c>
@@ -948,7 +948,7 @@
         <v>5630</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2020</v>
       </c>
@@ -968,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2020</v>
       </c>
@@ -988,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2020</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>271319</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2020</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>48408</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2020</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>1218102</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2020</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>272786</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2020</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>7498</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2020</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>36650</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2020</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>301822</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2020</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>9741</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2020</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>930837</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2019</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>496545</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2019</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>28570</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2019</v>
       </c>
@@ -1216,7 +1216,7 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2019</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>24309</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2019</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2019</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>228726</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2019</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2019</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>430086</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2019</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>10198</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2019</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>91596</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2019</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="31" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2019</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>16494</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2019</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2019</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>5630</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2019</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2019</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2019</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>231742</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2019</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>54012</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2019</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1138415</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2019</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>233486</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2019</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2019</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>35302</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2019</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>301842</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2019</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>9005</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2019</v>
       </c>
@@ -1638,18 +1638,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF74C8F-83D0-6746-93D5-463353E36558}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" s="2">
         <f>(Sheet1!F2+Sheet1!F7+Sheet1!F17)/(Sheet1!F21+Sheet1!F24+Sheet1!F22)</f>
         <v>0.93324583495102265</v>
@@ -1658,7 +1658,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <f>Sheet1!F9/SUM(Sheet1!F9:F12)</f>
         <v>0.80667239813795266</v>
@@ -1667,7 +1667,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <f>Sheet1!F10/SUM(Sheet1!F9:F12)</f>
         <v>1.9548897310726825E-2</v>
@@ -1676,7 +1676,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <f>Sheet1!F3/Sheet1!F2</f>
         <v>6.3064154601078337E-2</v>
@@ -1685,7 +1685,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <f>SUM(Sheet1!F9:F12)/Sheet1!F2</f>
         <v>1.165191823382288</v>
@@ -1694,7 +1694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <f>(Sheet1!F2-Sheet1!F27)/Sheet1!F27</f>
         <v>-6.9176006202861781E-2</v>
@@ -1716,14 +1716,14 @@
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="3.1640625" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1742,7 +1742,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>496545</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>28570</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>24309</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>228726</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>2748</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B11" s="10" t="s">
         <v>44</v>
       </c>
@@ -1833,11 +1833,11 @@
         <v>785472</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1845,7 +1845,7 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C14" s="8" t="s">
         <v>16</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>430086</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C15" s="8" t="s">
         <v>17</v>
       </c>
@@ -1867,7 +1867,7 @@
         <v>10198</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C16" s="8" t="s">
         <v>18</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>91596</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C17" s="8" t="s">
         <v>14</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>45</v>
       </c>
@@ -1903,14 +1903,14 @@
         <v>531881</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="26" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="26" x14ac:dyDescent="0.6">
       <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1918,7 +1918,7 @@
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="2:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:5" ht="31" x14ac:dyDescent="0.35">
       <c r="C22" s="13" t="s">
         <v>21</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>16494</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C23" s="8" t="s">
         <v>22</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C24" s="8" t="s">
         <v>23</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>5630</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C25" s="8" t="s">
         <v>24</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C26" s="14" t="s">
         <v>47</v>
       </c>
@@ -1975,7 +1975,7 @@
         <v>22309</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C27" s="8" t="s">
         <v>26</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C28" s="8" t="s">
         <v>27</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>231742</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C29" s="8" t="s">
         <v>28</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>54012</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C30" s="8" t="s">
         <v>29</v>
       </c>
@@ -2019,7 +2019,7 @@
         <v>1138415</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C31" s="14" t="s">
         <v>48</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>1424169</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" s="10" t="s">
         <v>49</v>
       </c>
@@ -2046,11 +2046,11 @@
         <v>1446478</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" s="5" t="s">
         <v>50</v>
       </c>
@@ -2058,7 +2058,7 @@
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C35" s="8" t="s">
         <v>32</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>233486</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C36" s="8" t="s">
         <v>33</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>2313</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C37" s="8" t="s">
         <v>34</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>35302</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C38" s="14" t="s">
         <v>51</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>271101</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C39" s="8" t="s">
         <v>36</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>301842</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C40" s="8" t="s">
         <v>37</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>9005</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C41" s="14" t="s">
         <v>52</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>310847</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="10" t="s">
         <v>53</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>581948</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" s="10" t="s">
         <v>38</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>864530</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C44" t="s">
         <v>54</v>
       </c>

</xml_diff>